<commit_message>
updated supplemental files for revision
</commit_message>
<xml_diff>
--- a/all_supp_files_first_submission/supp5_all_SP_drug_class_predictions.xlsx
+++ b/all_supp_files_first_submission/supp5_all_SP_drug_class_predictions.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenniferwilson/Documents/Designated-Medical-Event-Pathways/Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenniferwilson/Documents/Designated-Medical-Event-Pathways/all_supp_files_first_submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF0AAB1-2C6C-2C47-A193-A5C3355E460F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAA196A8-1C6B-A84A-A70E-3B6B056EF025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="660" windowWidth="25660" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18560" yWindow="1940" windowWidth="25660" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sort_table_SP" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$282</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sort_table_SP!$A$1:$F$282</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>

</xml_diff>